<commit_message>
Added a small helper for reading the indeces
</commit_message>
<xml_diff>
--- a/data/Mannschaft.xlsx
+++ b/data/Mannschaft.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,19 +424,19 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>Index</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Ordnungszahl</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Spielklasse</t>
-        </is>
-      </c>
       <c r="D1" t="inlineStr">
         <is>
           <t>Altersklasse</t>
@@ -449,1663 +449,1775 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Liganame</t>
+          <t>Mannschafts_ID</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Liganummer</t>
+          <t>Widget ID</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>Widget ID</t>
+          <t>Code groß</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>Code groß</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
           <t>Code klein</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> DJK SB München</t>
-        </is>
+      <c r="A2" t="n">
+        <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1</t>
+          <t xml:space="preserve"> DJK SB München</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t xml:space="preserve"> Senioren</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> männlich</t>
-        </is>
-      </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t xml:space="preserve"> männlich</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>152266</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>1733573700872</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t xml:space="preserve">&lt;div id="widget_1733573700872"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573700872',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"152266"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t xml:space="preserve">&lt;div id="widget_1733573700872"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573700872',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"152266"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t xml:space="preserve"> DJK SB München 2</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t xml:space="preserve"> 2</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t xml:space="preserve"> Senioren</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> männlich</t>
-        </is>
-      </c>
       <c r="E3" t="inlineStr">
         <is>
+          <t xml:space="preserve"> männlich</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>154153</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>1733573701194</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573701194"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573701194',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"154153"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573701194"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573701194',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"154153"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t xml:space="preserve"> DJK SB München 3</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t xml:space="preserve"> 3</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t xml:space="preserve"> Senioren</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> männlich</t>
-        </is>
-      </c>
       <c r="E4" t="inlineStr">
         <is>
+          <t xml:space="preserve"> männlich</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
           <t>163923</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>1733573701425</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573701425"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573701425',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"163923"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573701425"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573701425',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"163923"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t xml:space="preserve"> DJK SB München 4</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t xml:space="preserve"> 4</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t xml:space="preserve"> Senioren</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> männlich</t>
-        </is>
-      </c>
       <c r="E5" t="inlineStr">
         <is>
+          <t xml:space="preserve"> männlich</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>163914</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>1733573701687</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573701687"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573701687',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"163914"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573701687"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573701687',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"163914"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> DJK SB München</t>
-        </is>
+      <c r="A6" t="n">
+        <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1</t>
+          <t xml:space="preserve"> DJK SB München</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t xml:space="preserve"> U18</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> männlich</t>
-        </is>
-      </c>
       <c r="E6" t="inlineStr">
         <is>
+          <t xml:space="preserve"> männlich</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
           <t>162955</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>1733573701932</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573701932"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573701932',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"162955"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573701932"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573701932',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"162955"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> DJK SB München</t>
-        </is>
+      <c r="A7" t="n">
+        <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t xml:space="preserve"> DJK SB München</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t xml:space="preserve"> 2</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t xml:space="preserve"> U18</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> männlich</t>
-        </is>
-      </c>
       <c r="E7" t="inlineStr">
         <is>
+          <t xml:space="preserve"> männlich</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
           <t>223272</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>1733573702146</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573702146"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573702146',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"223272"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573702146"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573702146',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"223272"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> DJK SB München</t>
-        </is>
+      <c r="A8" t="n">
+        <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1</t>
+          <t xml:space="preserve"> DJK SB München</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t xml:space="preserve"> U16</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> männlich</t>
-        </is>
-      </c>
       <c r="E8" t="inlineStr">
         <is>
+          <t xml:space="preserve"> männlich</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
           <t>166180</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>1733573702359</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573702359"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573702359',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"166180"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573702359"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573702359',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"166180"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t xml:space="preserve"> DJK SB München 2</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t xml:space="preserve"> 2</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t xml:space="preserve"> U16</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> männlich</t>
-        </is>
-      </c>
       <c r="E9" t="inlineStr">
         <is>
+          <t xml:space="preserve"> männlich</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
           <t>162996</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="G9" t="inlineStr">
         <is>
           <t>1733573702568</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573702568"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573702568',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"162996"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573702568"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573702568',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"162996"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t xml:space="preserve"> DJK SB München 3</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t xml:space="preserve"> 3</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t xml:space="preserve"> U16</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> männlich</t>
-        </is>
-      </c>
       <c r="E10" t="inlineStr">
         <is>
+          <t xml:space="preserve"> männlich</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
           <t>309729</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>1733573702768</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573702768"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573702768',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"309729"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573702768"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573702768',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"309729"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> DJK SB München</t>
-        </is>
+      <c r="A11" t="n">
+        <v>9</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1</t>
+          <t xml:space="preserve"> DJK SB München</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t xml:space="preserve"> U16</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t xml:space="preserve"> weiblich</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>319500</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>1733573702946</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573702946"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573702946',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"319500"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573702946"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573702946',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"319500"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> DJK SB München</t>
-        </is>
+      <c r="A12" t="n">
+        <v>10</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1</t>
+          <t xml:space="preserve"> DJK SB München</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
           <t xml:space="preserve"> U14</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> männlich</t>
-        </is>
-      </c>
       <c r="E12" t="inlineStr">
         <is>
+          <t xml:space="preserve"> männlich</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
           <t>165708</t>
         </is>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>1733573703126</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573703126"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573703126',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"165708"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573703126"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573703126',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"165708"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t xml:space="preserve"> DJK SB München 2</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t xml:space="preserve"> 2</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t xml:space="preserve"> U14</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> männlich</t>
-        </is>
-      </c>
       <c r="E13" t="inlineStr">
         <is>
+          <t xml:space="preserve"> männlich</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
           <t>163006</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>1733573703306</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573703306"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573703306',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"163006"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573703306"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573703306',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"163006"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t xml:space="preserve"> DJK SB München 3</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t xml:space="preserve"> 3</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t xml:space="preserve"> U14</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> männlich</t>
-        </is>
-      </c>
       <c r="E14" t="inlineStr">
         <is>
+          <t xml:space="preserve"> männlich</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
           <t>314794</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>1733573703486</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573703486"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573703486',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"314794"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573703486"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573703486',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"314794"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> DJK SB München</t>
-        </is>
+      <c r="A15" t="n">
+        <v>13</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1</t>
+          <t xml:space="preserve"> DJK SB München</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
           <t xml:space="preserve"> U14</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t xml:space="preserve"> weiblich</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>317459</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>1733573703674</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573703674"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573703674',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"317459"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573703674"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573703674',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"317459"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
         <is>
           <t xml:space="preserve"> DJK SB München 2</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t xml:space="preserve"> 2</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t xml:space="preserve"> U14</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t xml:space="preserve"> weiblich</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>317505</t>
         </is>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>1733573703861</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573703861"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573703861',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"317505"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573703861"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573703861',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"317505"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> DJK SB München</t>
-        </is>
+      <c r="A17" t="n">
+        <v>15</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1</t>
+          <t xml:space="preserve"> DJK SB München</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
           <t xml:space="preserve"> U12</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> männlich</t>
-        </is>
-      </c>
       <c r="E17" t="inlineStr">
         <is>
+          <t xml:space="preserve"> männlich</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
           <t>162748</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="G17" t="inlineStr">
         <is>
           <t>1733573704047</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573704047"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573704047',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"162748"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="I17" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573704047"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573704047',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"162748"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
         <is>
           <t xml:space="preserve"> DJK SB München 2</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t xml:space="preserve"> 2</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t xml:space="preserve"> U12</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> männlich</t>
-        </is>
-      </c>
       <c r="E18" t="inlineStr">
         <is>
+          <t xml:space="preserve"> männlich</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
           <t>310490</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>1733573704230</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573704230"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573704230',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"310490"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="I18" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573704230"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573704230',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"310490"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> DJK SB München</t>
-        </is>
+      <c r="A19" t="n">
+        <v>17</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1</t>
+          <t xml:space="preserve"> DJK SB München</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
           <t xml:space="preserve"> U12</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t xml:space="preserve"> weiblich</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>316293</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="G19" t="inlineStr">
         <is>
           <t>1733573704425</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="H19" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573704425"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573704425',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"316293"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="I19" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573704425"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573704425',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"316293"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> DJK SB München</t>
-        </is>
+      <c r="A20" t="n">
+        <v>18</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1</t>
+          <t xml:space="preserve"> DJK SB München</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
           <t xml:space="preserve"> U10</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> männlich</t>
-        </is>
-      </c>
       <c r="E20" t="inlineStr">
         <is>
+          <t xml:space="preserve"> männlich</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
           <t>310512</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="G20" t="inlineStr">
         <is>
           <t>1733573704614</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="H20" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573704614"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573704614',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"310512"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="I20" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573704614"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573704614',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"310512"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> DJK SB München</t>
-        </is>
+      <c r="A21" t="n">
+        <v>19</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t xml:space="preserve"> DJK SB München</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
           <t xml:space="preserve"> 2</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t xml:space="preserve"> U10</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> männlich</t>
-        </is>
-      </c>
       <c r="E21" t="inlineStr">
         <is>
+          <t xml:space="preserve"> männlich</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
           <t>313178</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="G21" t="inlineStr">
         <is>
           <t>1733573704799</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="H21" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573704799"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573704799',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"313178"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H21" t="inlineStr">
+      <c r="I21" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573704799"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573704799',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"313178"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> DJK SB München</t>
-        </is>
+      <c r="A22" t="n">
+        <v>20</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1</t>
+          <t xml:space="preserve"> DJK SB München</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
           <t xml:space="preserve"> U10</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t xml:space="preserve"> weiblich</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>317910</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="G22" t="inlineStr">
         <is>
           <t>1733573704997</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
+      <c r="H22" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573704997"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573704997',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"317910"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H22" t="inlineStr">
+      <c r="I22" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573704997"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573704997',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"317910"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> DJK SB München</t>
-        </is>
+      <c r="A23" t="n">
+        <v>21</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1</t>
+          <t xml:space="preserve"> DJK SB München</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
           <t xml:space="preserve"> Ü40</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> männlich</t>
-        </is>
-      </c>
       <c r="E23" t="inlineStr">
         <is>
+          <t xml:space="preserve"> männlich</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
           <t>165461</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="G23" t="inlineStr">
         <is>
           <t>1733573705209</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="H23" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573705209"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573705209',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"165461"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H23" t="inlineStr">
+      <c r="I23" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573705209"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573705209',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"165461"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> DJK SB München</t>
-        </is>
+      <c r="A24" t="n">
+        <v>22</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1</t>
+          <t xml:space="preserve"> DJK SB München</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
           <t xml:space="preserve"> Ü40</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t xml:space="preserve"> mix</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr">
+      <c r="F24" t="inlineStr">
         <is>
           <t>223249</t>
         </is>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="G24" t="inlineStr">
         <is>
           <t>1733573705406</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="H24" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573705406"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573705406',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"223249"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H24" t="inlineStr">
+      <c r="I24" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573705406"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573705406',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"223249"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> DJK SB München</t>
-        </is>
+      <c r="A25" t="n">
+        <v>23</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1</t>
+          <t xml:space="preserve"> DJK SB München</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
           <t xml:space="preserve"> Ü35</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> männlich</t>
-        </is>
-      </c>
       <c r="E25" t="inlineStr">
         <is>
+          <t xml:space="preserve"> männlich</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
           <t>311561</t>
         </is>
       </c>
-      <c r="F25" t="inlineStr">
+      <c r="G25" t="inlineStr">
         <is>
           <t>1733573705600</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
+      <c r="H25" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573705600"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573705600',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"311561"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H25" t="inlineStr">
+      <c r="I25" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573705600"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573705600',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"311561"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> DJK SB München</t>
-        </is>
+      <c r="A26" t="n">
+        <v>24</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1</t>
+          <t xml:space="preserve"> DJK SB München</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
           <t xml:space="preserve"> Senioren</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="E26" t="inlineStr">
         <is>
           <t xml:space="preserve"> weiblich</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="F26" t="inlineStr">
         <is>
           <t>223146</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="G26" t="inlineStr">
         <is>
           <t>1733573705815</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
+      <c r="H26" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573705815"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573705815',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"223146"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H26" t="inlineStr">
+      <c r="I26" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573705815"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573705815',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"223146"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> DJK SB München</t>
-        </is>
+      <c r="A27" t="n">
+        <v>25</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1</t>
+          <t xml:space="preserve"> DJK SB München</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
           <t xml:space="preserve"> U20</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> männlich</t>
-        </is>
-      </c>
       <c r="E27" t="inlineStr">
         <is>
+          <t xml:space="preserve"> männlich</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
           <t>223247</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr">
+      <c r="G27" t="inlineStr">
         <is>
           <t>1733573706050</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr">
+      <c r="H27" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573706050"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573706050',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"223247"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H27" t="inlineStr">
+      <c r="I27" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573706050"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573706050',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"223247"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> DJK SB München</t>
-        </is>
+      <c r="A28" t="n">
+        <v>26</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1</t>
+          <t xml:space="preserve"> DJK SB München</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
           <t xml:space="preserve"> U18</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="E28" t="inlineStr">
         <is>
           <t xml:space="preserve"> weiblich</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="F28" t="inlineStr">
         <is>
           <t>223246</t>
         </is>
       </c>
-      <c r="F28" t="inlineStr">
+      <c r="G28" t="inlineStr">
         <is>
           <t>1733573706258</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr">
+      <c r="H28" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573706258"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573706258',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"223246"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H28" t="inlineStr">
+      <c r="I28" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573706258"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573706258',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"223246"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
+      <c r="A29" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
         <is>
           <t xml:space="preserve"> DJK SB München 2 u18BZLQuali</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1</t>
-        </is>
-      </c>
       <c r="C29" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
           <t xml:space="preserve"> U17</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> männlich</t>
-        </is>
-      </c>
       <c r="E29" t="inlineStr">
         <is>
+          <t xml:space="preserve"> männlich</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
           <t>312003</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr">
+      <c r="G29" t="inlineStr">
         <is>
           <t>1733573706447</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
+      <c r="H29" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573706447"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573706447',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"312003"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H29" t="inlineStr">
+      <c r="I29" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573706447"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573706447',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"312003"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> DJK SB München</t>
-        </is>
+      <c r="A30" t="n">
+        <v>28</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1</t>
+          <t xml:space="preserve"> DJK SB München</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
           <t xml:space="preserve"> U16</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="E30" t="inlineStr">
         <is>
           <t xml:space="preserve"> mix</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr">
+      <c r="F30" t="inlineStr">
         <is>
           <t>223221</t>
         </is>
       </c>
-      <c r="F30" t="inlineStr">
+      <c r="G30" t="inlineStr">
         <is>
           <t>1733573706631</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr">
+      <c r="H30" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573706631"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573706631',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"223221"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H30" t="inlineStr">
+      <c r="I30" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573706631"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573706631',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"223221"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> DJK SB München</t>
-        </is>
+      <c r="A31" t="n">
+        <v>29</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1</t>
+          <t xml:space="preserve"> DJK SB München</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
           <t xml:space="preserve"> U15</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> männlich</t>
-        </is>
-      </c>
       <c r="E31" t="inlineStr">
         <is>
+          <t xml:space="preserve"> männlich</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
           <t>310694</t>
         </is>
       </c>
-      <c r="F31" t="inlineStr">
+      <c r="G31" t="inlineStr">
         <is>
           <t>1733573706838</t>
         </is>
       </c>
-      <c r="G31" t="inlineStr">
+      <c r="H31" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573706838"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573706838',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"310694"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H31" t="inlineStr">
+      <c r="I31" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573706838"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573706838',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"310694"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
+      <c r="A32" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
         <is>
           <t xml:space="preserve"> DJK SB München 2 -Quali BOL16</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="C32" t="inlineStr">
         <is>
           <t xml:space="preserve"> 2</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t xml:space="preserve"> U15</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> männlich</t>
-        </is>
-      </c>
       <c r="E32" t="inlineStr">
         <is>
+          <t xml:space="preserve"> männlich</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
           <t>317441</t>
         </is>
       </c>
-      <c r="F32" t="inlineStr">
+      <c r="G32" t="inlineStr">
         <is>
           <t>1733573707077</t>
         </is>
       </c>
-      <c r="G32" t="inlineStr">
+      <c r="H32" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573707077"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573707077',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"317441"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H32" t="inlineStr">
+      <c r="I32" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573707077"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573707077',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"317441"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> DJK SB München</t>
-        </is>
+      <c r="A33" t="n">
+        <v>31</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
+          <t xml:space="preserve"> DJK SB München</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
           <t xml:space="preserve"> 2</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="D33" t="inlineStr">
         <is>
           <t xml:space="preserve"> U14</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="E33" t="inlineStr">
         <is>
           <t xml:space="preserve"> mix</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr">
+      <c r="F33" t="inlineStr">
         <is>
           <t>223269</t>
         </is>
       </c>
-      <c r="F33" t="inlineStr">
+      <c r="G33" t="inlineStr">
         <is>
           <t>1733573707272</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr">
+      <c r="H33" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573707272"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573707272',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"223269"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H33" t="inlineStr">
+      <c r="I33" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573707272"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573707272',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"223269"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> DJK SB München</t>
-        </is>
+      <c r="A34" t="n">
+        <v>32</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1</t>
+          <t xml:space="preserve"> DJK SB München</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
           <t xml:space="preserve"> U13</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> männlich</t>
-        </is>
-      </c>
       <c r="E34" t="inlineStr">
         <is>
+          <t xml:space="preserve"> männlich</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
           <t>311924</t>
         </is>
       </c>
-      <c r="F34" t="inlineStr">
+      <c r="G34" t="inlineStr">
         <is>
           <t>1733573707460</t>
         </is>
       </c>
-      <c r="G34" t="inlineStr">
+      <c r="H34" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573707460"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573707460',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"311924"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H34" t="inlineStr">
+      <c r="I34" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573707460"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573707460',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"311924"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> DJK SB München</t>
-        </is>
+      <c r="A35" t="n">
+        <v>33</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1</t>
+          <t xml:space="preserve"> DJK SB München</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
           <t xml:space="preserve"> U12</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="E35" t="inlineStr">
         <is>
           <t xml:space="preserve"> mix</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr">
+      <c r="F35" t="inlineStr">
         <is>
           <t>223172</t>
         </is>
       </c>
-      <c r="F35" t="inlineStr">
+      <c r="G35" t="inlineStr">
         <is>
           <t>1733573707667</t>
         </is>
       </c>
-      <c r="G35" t="inlineStr">
+      <c r="H35" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573707667"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573707667',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"223172"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H35" t="inlineStr">
+      <c r="I35" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573707667"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573707667',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"223172"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
+      <c r="A36" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
         <is>
           <t xml:space="preserve"> DJK SB München 2</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="C36" t="inlineStr">
         <is>
           <t xml:space="preserve"> 2</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="D36" t="inlineStr">
         <is>
           <t xml:space="preserve"> U12</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="E36" t="inlineStr">
         <is>
           <t xml:space="preserve"> mix</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
+      <c r="F36" t="inlineStr">
         <is>
           <t>223264</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr">
+      <c r="G36" t="inlineStr">
         <is>
           <t>1733573707904</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr">
+      <c r="H36" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573707904"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573707904',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"223264"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H36" t="inlineStr">
+      <c r="I36" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573707904"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573707904',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"223264"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
+      <c r="A37" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
         <is>
           <t xml:space="preserve"> DJK SB München 2 u12BZLQuali</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 1</t>
-        </is>
-      </c>
       <c r="C37" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
           <t xml:space="preserve"> U11</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> männlich</t>
-        </is>
-      </c>
       <c r="E37" t="inlineStr">
         <is>
+          <t xml:space="preserve"> männlich</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
           <t>311982</t>
         </is>
       </c>
-      <c r="F37" t="inlineStr">
+      <c r="G37" t="inlineStr">
         <is>
           <t>1733573708108</t>
         </is>
       </c>
-      <c r="G37" t="inlineStr">
+      <c r="H37" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573708108"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573708108',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"311982"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H37" t="inlineStr">
+      <c r="I37" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573708108"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573708108',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"311982"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> DJK SB München</t>
-        </is>
+      <c r="A38" t="n">
+        <v>36</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1</t>
+          <t xml:space="preserve"> DJK SB München</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
           <t xml:space="preserve"> U10</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="E38" t="inlineStr">
         <is>
           <t xml:space="preserve"> mix</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
+      <c r="F38" t="inlineStr">
         <is>
           <t>165490</t>
         </is>
       </c>
-      <c r="F38" t="inlineStr">
+      <c r="G38" t="inlineStr">
         <is>
           <t>1733573708301</t>
         </is>
       </c>
-      <c r="G38" t="inlineStr">
+      <c r="H38" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573708301"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573708301',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"165490"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H38" t="inlineStr">
+      <c r="I38" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573708301"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573708301',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"165490"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> DJK SB München</t>
-        </is>
+      <c r="A39" t="n">
+        <v>37</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1</t>
+          <t xml:space="preserve"> DJK SB München</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
           <t xml:space="preserve"> U8</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> männlich</t>
-        </is>
-      </c>
       <c r="E39" t="inlineStr">
         <is>
+          <t xml:space="preserve"> männlich</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
           <t>310167</t>
         </is>
       </c>
-      <c r="F39" t="inlineStr">
+      <c r="G39" t="inlineStr">
         <is>
           <t>1733573708488</t>
         </is>
       </c>
-      <c r="G39" t="inlineStr">
+      <c r="H39" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573708488"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573708488',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"310167"} );     &lt;/script&gt;     </t>
         </is>
       </c>
-      <c r="H39" t="inlineStr">
+      <c r="I39" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573708488"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573708488',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"310167"} );     &lt;/script&gt;     </t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> DJK SB München</t>
-        </is>
+      <c r="A40" t="n">
+        <v>38</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1</t>
+          <t xml:space="preserve"> DJK SB München</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
+          <t xml:space="preserve"> 1</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
           <t xml:space="preserve"> U8</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="E40" t="inlineStr">
         <is>
           <t xml:space="preserve"> mix</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr">
+      <c r="F40" t="inlineStr">
         <is>
           <t>165491</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr">
+      <c r="G40" t="inlineStr">
         <is>
           <t>1733573708690</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr">
+      <c r="H40" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573708690"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573708690',             {"iframeWidth":1200,"iframeHeight":600,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"165491"} );     &lt;/script&gt;</t>
         </is>
       </c>
-      <c r="H40" t="inlineStr">
+      <c r="I40" t="inlineStr">
         <is>
           <t xml:space="preserve">    &lt;div id="widget_1733573708690"&gt;&lt;/div&gt;     &lt;script&gt;         widget.mannschaftswidget('widget_1733573708690',             {"iframeWidth":600,"iframeHeight":700,"showRefreshButton":false,"titleColor":"FFFFFF","titleBgColor":"00CC00","tapColor":"FFFFFF","tapBgColor":"333333","colorMatchGroup":"666666","bgColorMatchGroup":"F0F0F0","colorMatchListItem":"000000","bgColorMatchListItem":"FFFFFF","showKuerzelInSpiele":false,"mannschaftsId":"165491"} );     &lt;/script&gt;</t>
         </is>

</xml_diff>